<commit_message>
Reorganise images, update README
Add pinout and dimension images, add to readme, rename files, tidy.
</commit_message>
<xml_diff>
--- a/Source/Outputs/RUMBA_plus_v1_4_2A_BOM.xlsx
+++ b/Source/Outputs/RUMBA_plus_v1_4_2A_BOM.xlsx
@@ -1,23 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Git\RUMBA-Plus\Source\Outputs\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7E7A7B84-4C35-4740-B479-7AB09EEFDAA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{69699B33-CDB8-42D2-925A-EB59F2C058E0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1515" yWindow="1515" windowWidth="21600" windowHeight="12735" xr2:uid="{687194B3-0182-4A23-8F2D-914AF6B11412}"/>
+    <workbookView xWindow="1035" yWindow="1035" windowWidth="4110" windowHeight="10725" xr2:uid="{E70BCA24-BCAC-4C8A-8492-EE748680D711}"/>
   </bookViews>
   <sheets>
-    <sheet name="RUMBA_plus_v1_4_2A_BOM" sheetId="1" r:id="rId1"/>
+    <sheet name="RUMBA_plus_1_4_2A_BOM" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">RUMBA_plus_v1_4_2A_BOM!$1:$1</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -26,9 +18,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="216">
   <si>
     <t>Designator</t>
   </si>
@@ -170,7 +160,7 @@
     <t>Kyocera AVX</t>
   </si>
   <si>
-    <t>06035C220JAT2A\4K</t>
+    <t>06035C220JAT2A</t>
   </si>
   <si>
     <t>478-6204-1-ND</t>
@@ -200,7 +190,7 @@
     <t>Epson</t>
   </si>
   <si>
-    <t>FA-23816.0000MB-C3</t>
+    <t>FA-23816.0000MBC3</t>
   </si>
   <si>
     <t>SER3686CT-ND</t>
@@ -257,7 +247,7 @@
     <t>DIODE SCHOTTKY 40V 4A DO214AA</t>
   </si>
   <si>
-    <t>Vishay Semiconductors</t>
+    <t>General Instruments</t>
   </si>
   <si>
     <t>SSB44-E3/52T</t>
@@ -332,6 +322,9 @@
     <t>Generic Header</t>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
     <t>VFA0_sel, VFA1_sel, VHE2_sel, X-, X+, Y-, Y+, Z-, Z+</t>
   </si>
   <si>
@@ -380,21 +373,24 @@
     <t>IC MCU 8BIT 16KB FLASH 32VQFN</t>
   </si>
   <si>
+    <t>Microchip</t>
+  </si>
+  <si>
+    <t>ATMEGA16U2-MU</t>
+  </si>
+  <si>
+    <t>ATMEGA16U2-MU-ND</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>IC MCU 8BIT 256KB FLASH 100TQFP</t>
+  </si>
+  <si>
     <t>Microchip / Atmel</t>
   </si>
   <si>
-    <t>ATMEGA16U2-MU</t>
-  </si>
-  <si>
-    <t>ATMEGA16U2-MU-ND</t>
-  </si>
-  <si>
-    <t>U1</t>
-  </si>
-  <si>
-    <t>IC MCU 8BIT 256KB FLASH 100TQFP</t>
-  </si>
-  <si>
     <t>ATMEGA2560-16AU</t>
   </si>
   <si>
@@ -488,7 +484,7 @@
     <t>PTC RESET FUSE 9V 200MA 0603</t>
   </si>
   <si>
-    <t>BEL FUSE - CIRCUIT PROTECTION</t>
+    <t>Bel</t>
   </si>
   <si>
     <t>0ZCM0020FF2G</t>
@@ -527,21 +523,21 @@
     <t>RES SMD 4.7K OHM 1% 1/10W 0603</t>
   </si>
   <si>
+    <t>RC0603FR-074K7L</t>
+  </si>
+  <si>
+    <t>311-4.70KHRCT-ND</t>
+  </si>
+  <si>
+    <t>R2, R3, R6, R11, R12, R21, R23, R25, R27, R29, R45, R57</t>
+  </si>
+  <si>
+    <t>RES SMD 10K OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
     <t>Yageo Phycomp</t>
   </si>
   <si>
-    <t>RC0603FR-074K7L</t>
-  </si>
-  <si>
-    <t>311-4.70KHRCT-ND</t>
-  </si>
-  <si>
-    <t>R2, R3, R6, R11, R12, R21, R23, R25, R27, R29, R45, R57</t>
-  </si>
-  <si>
-    <t>RES SMD 10K OHM 1% 1/10W 0603</t>
-  </si>
-  <si>
     <t>RC0603FR-0710KL</t>
   </si>
   <si>
@@ -635,7 +631,7 @@
     <t>Phoenix Contact</t>
   </si>
   <si>
-    <t>1751248</t>
+    <t>MKDS1/2-3,5</t>
   </si>
   <si>
     <t>277-5719-ND</t>
@@ -647,9 +643,6 @@
     <t>TERM BLK 2POS SIDE ENTRY 5MM PCB</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>1935776</t>
   </si>
   <si>
@@ -662,7 +655,7 @@
     <t>TERM BLK 4POS SIDE ENT 3.5MM PCB</t>
   </si>
   <si>
-    <t>1751264</t>
+    <t>MKDS1/4-3,5</t>
   </si>
   <si>
     <t>277-5744-ND</t>
@@ -687,10 +680,24 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -705,7 +712,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFD3D3D3"/>
+        <fgColor indexed="22"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -734,23 +741,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1062,1243 +1067,1445 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C12E5BAD-049D-4374-A6F3-A76AD96DDFBC}">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A310E97-4643-4F2C-A7EF-E3FEC2F4018E}">
   <dimension ref="A1:H49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="92.42578125" customWidth="1"/>
-    <col min="2" max="2" width="44.7109375" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" customWidth="1"/>
-    <col min="4" max="4" width="45.5703125" customWidth="1"/>
-    <col min="5" max="5" width="33.85546875" customWidth="1"/>
-    <col min="6" max="6" width="29.85546875" customWidth="1"/>
-    <col min="7" max="7" width="12" customWidth="1"/>
-    <col min="8" max="8" width="33.42578125" customWidth="1"/>
+    <col min="1" max="1" width="35.28515625" customWidth="1"/>
+    <col min="2" max="2" width="37.140625" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
+    <col min="6" max="6" width="20.5703125" customWidth="1"/>
+    <col min="7" max="7" width="23.140625" customWidth="1"/>
+    <col min="8" max="8" width="26.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="3">
         <v>3</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="3" t="s">
+      <c r="G2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <v>9</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="3" t="s">
+      <c r="D3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" s="3" t="s">
+      <c r="G3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="3">
         <v>11</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="3" t="s">
+      <c r="D4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="3" t="s">
+      <c r="G4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="4" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="3">
         <v>6</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="3" t="s">
+      <c r="D5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="G5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H5" s="3" t="s">
+      <c r="G5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="4" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="3">
         <v>2</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="3" t="s">
+      <c r="D6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="G6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H6" s="3" t="s">
+      <c r="G6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="4" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="3">
         <v>3</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="3" t="s">
+      <c r="D7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="G7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H7" s="3" t="s">
+      <c r="G7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="4" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="3">
         <v>5</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" s="3" t="s">
+      <c r="D8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="G8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H8" s="3" t="s">
+      <c r="G8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="4" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="3">
         <v>1</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="3" t="s">
+      <c r="D9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="G9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H9" s="3" t="s">
+      <c r="G9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="4" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="3">
         <v>2</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10" s="3" t="s">
+      <c r="D10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="G10" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H10" s="3" t="s">
+      <c r="G10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" s="4" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="3">
         <v>2</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" s="3" t="s">
+      <c r="D11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="G11" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H11" s="3" t="s">
+      <c r="G11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H11" s="4" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="3">
         <v>8</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" s="3" t="s">
+      <c r="D12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="G12" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H12" s="3" t="s">
+      <c r="G12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H12" s="4" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="3">
         <v>3</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E13" s="3" t="s">
+      <c r="D13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F13" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="G13" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H13" s="3" t="s">
+      <c r="G13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H13" s="4" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14" s="3">
         <v>1</v>
       </c>
-      <c r="D14" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E14" s="3" t="s">
+      <c r="D14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F14" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="G14" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H14" s="3" t="s">
+      <c r="G14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H14" s="4" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="3">
         <v>1</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E15" s="3" t="s">
+      <c r="D15" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="F15" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="G15" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H15" s="3" t="s">
+      <c r="G15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H15" s="4" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16" s="3">
         <v>1</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E16" s="3" t="s">
+      <c r="D16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="F16" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="G16" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H16" s="3" t="s">
+      <c r="G16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H16" s="4" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17" s="3">
         <v>1</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E17" s="3" t="s">
+      <c r="D17" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="F17" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="G17" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H17" s="3" t="s">
+      <c r="G17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H17" s="4" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18" s="3">
         <v>2</v>
       </c>
-      <c r="D18" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E18" s="3" t="s">
+      <c r="D18" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="F18" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="G18" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H18" s="3" t="s">
+      <c r="G18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H18" s="4" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="C19" s="4">
+      <c r="C19" s="3">
         <v>6</v>
       </c>
-      <c r="D19" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E19" s="3" t="s">
+      <c r="D19" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
+      <c r="F19" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="B20" s="3" t="s">
+      <c r="A20" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="C20" s="4">
+      <c r="B20" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C20" s="3">
         <v>9</v>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E20" s="3" t="s">
+      <c r="D20" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E20" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
+      <c r="F20" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="B21" s="3" t="s">
+      <c r="A21" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C21" s="4">
+      <c r="B21" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C21" s="3">
         <v>2</v>
       </c>
-      <c r="D21" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E21" s="3" t="s">
+      <c r="D21" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
+      <c r="F21" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="B22" s="3" t="s">
+      <c r="A22" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C22" s="4">
+      <c r="B22" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C22" s="3">
         <v>10</v>
       </c>
-      <c r="D22" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E22" s="3" t="s">
+      <c r="D22" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E22" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
+      <c r="F22" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="B23" s="3" t="s">
+      <c r="A23" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="C23" s="4">
+      <c r="B23" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C23" s="3">
         <v>1</v>
       </c>
-      <c r="D23" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E23" s="3" t="s">
+      <c r="D23" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E23" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
+      <c r="F23" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="B24" s="3" t="s">
+      <c r="A24" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C24" s="4">
+      <c r="B24" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C24" s="3">
         <v>4</v>
       </c>
-      <c r="D24" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E24" s="3" t="s">
+      <c r="D24" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E24" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
+      <c r="F24" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="B25" s="3" t="s">
+      <c r="A25" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="C25" s="4">
+      <c r="B25" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C25" s="3">
         <v>1</v>
       </c>
-      <c r="D25" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E25" s="3" t="s">
+      <c r="D25" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E25" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
+      <c r="F25" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="B26" s="3" t="s">
+      <c r="A26" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="C26" s="4">
+      <c r="B26" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C26" s="3">
         <v>12</v>
       </c>
-      <c r="D26" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E26" s="3" t="s">
+      <c r="D26" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E26" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
+      <c r="F26" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="B27" s="3" t="s">
+      <c r="A27" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="C27" s="4">
+      <c r="B27" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C27" s="3">
         <v>1</v>
       </c>
-      <c r="D27" s="4"/>
-      <c r="E27" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="F27" s="3" t="s">
+      <c r="D27" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E27" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="G27" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H27" s="3" t="s">
+      <c r="F27" s="4" t="s">
         <v>116</v>
       </c>
+      <c r="G27" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="B28" s="3" t="s">
+      <c r="A28" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="C28" s="4">
+      <c r="B28" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C28" s="3">
         <v>1</v>
       </c>
-      <c r="D28" s="4"/>
-      <c r="E28" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H28" s="3" t="s">
+      <c r="D28" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E28" s="4" t="s">
         <v>120</v>
       </c>
+      <c r="F28" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="C29" s="4">
+      <c r="A29" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C29" s="3">
         <v>1</v>
       </c>
-      <c r="D29" s="4"/>
-      <c r="E29" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="G29" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H29" s="3" t="s">
+      <c r="D29" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E29" s="4" t="s">
         <v>125</v>
       </c>
+      <c r="F29" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="C30" s="4">
+      <c r="A30" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C30" s="3">
         <v>1</v>
       </c>
-      <c r="D30" s="4"/>
-      <c r="E30" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="G30" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H30" s="3" t="s">
-        <v>129</v>
+      <c r="D30" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="C31" s="4">
+      <c r="A31" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C31" s="3">
         <v>10</v>
       </c>
-      <c r="D31" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="G31" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H31" s="3" t="s">
+      <c r="D31" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E31" s="4" t="s">
         <v>134</v>
       </c>
+      <c r="F31" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="C32" s="4">
+      <c r="A32" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C32" s="3">
         <v>3</v>
       </c>
-      <c r="D32" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="G32" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H32" s="3" t="s">
-        <v>138</v>
+      <c r="D32" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H32" s="4" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="C33" s="4">
+      <c r="A33" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C33" s="3">
         <v>5</v>
       </c>
-      <c r="D33" s="4"/>
-      <c r="E33" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="G33" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H33" s="3" t="s">
+      <c r="D33" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E33" s="4" t="s">
         <v>143</v>
       </c>
+      <c r="F33" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H33" s="4" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="C34" s="4">
+      <c r="A34" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C34" s="3">
         <v>1</v>
       </c>
-      <c r="D34" s="4"/>
-      <c r="E34" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="G34" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H34" s="3" t="s">
-        <v>147</v>
+      <c r="D34" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H34" s="4" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="C35" s="4">
+      <c r="A35" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C35" s="3">
         <v>1</v>
       </c>
-      <c r="D35" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="F35" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="G35" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H35" s="3" t="s">
+      <c r="D35" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E35" s="4" t="s">
         <v>152</v>
       </c>
+      <c r="F35" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H35" s="4" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="C36" s="4">
+      <c r="A36" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C36" s="3">
         <v>15</v>
       </c>
-      <c r="D36" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E36" s="3" t="s">
+      <c r="D36" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E36" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F36" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="G36" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H36" s="3" t="s">
-        <v>156</v>
+      <c r="F36" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H36" s="4" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="C37" s="4">
+      <c r="A37" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C37" s="3">
         <v>2</v>
       </c>
-      <c r="D37" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E37" s="3" t="s">
+      <c r="D37" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E37" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F37" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="G37" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H37" s="3" t="s">
-        <v>160</v>
+      <c r="F37" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H37" s="4" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="C38" s="4">
+      <c r="A38" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C38" s="3">
         <v>6</v>
       </c>
-      <c r="D38" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="F38" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="G38" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H38" s="3" t="s">
+      <c r="D38" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F38" s="4" t="s">
         <v>165</v>
       </c>
+      <c r="G38" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H38" s="4" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="B39" s="3" t="s">
+      <c r="A39" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="C39" s="4">
+      <c r="B39" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C39" s="3">
         <v>12</v>
       </c>
-      <c r="D39" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="F39" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="G39" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H39" s="3" t="s">
+      <c r="D39" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E39" s="4" t="s">
         <v>169</v>
       </c>
+      <c r="F39" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H39" s="4" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="C40" s="4">
+      <c r="A40" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="C40" s="3">
         <v>8</v>
       </c>
-      <c r="D40" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E40" s="3" t="s">
+      <c r="D40" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E40" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F40" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="G40" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H40" s="3" t="s">
-        <v>173</v>
+      <c r="F40" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H40" s="4" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="C41" s="4">
+      <c r="A41" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C41" s="3">
         <v>2</v>
       </c>
-      <c r="D41" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E41" s="3" t="s">
+      <c r="D41" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E41" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F41" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="G41" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H41" s="3" t="s">
-        <v>177</v>
+      <c r="F41" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H41" s="4" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="C42" s="4">
-        <v>13</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E42" s="3" t="s">
+      <c r="A42" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C42" s="3">
+        <v>13</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E42" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F42" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="G42" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H42" s="3" t="s">
-        <v>181</v>
+      <c r="F42" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H42" s="4" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="C43" s="4">
+      <c r="A43" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="C43" s="3">
         <v>1</v>
       </c>
-      <c r="D43" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E43" s="3" t="s">
+      <c r="D43" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E43" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F43" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="G43" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H43" s="3" t="s">
-        <v>185</v>
+      <c r="F43" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H43" s="4" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="C44" s="4">
+      <c r="A44" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C44" s="3">
         <v>6</v>
       </c>
-      <c r="D44" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E44" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="F44" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="G44" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H44" s="3" t="s">
+      <c r="D44" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E44" s="4" t="s">
         <v>190</v>
       </c>
+      <c r="F44" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H44" s="4" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="C45" s="4">
+      <c r="A45" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="C45" s="3">
         <v>1</v>
       </c>
-      <c r="D45" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E45" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="F45" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="G45" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H45" s="3" t="s">
+      <c r="D45" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E45" s="4" t="s">
         <v>195</v>
       </c>
+      <c r="F45" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H45" s="4" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="C46" s="4">
+      <c r="A46" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="C46" s="3">
         <v>5</v>
       </c>
-      <c r="D46" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E46" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="F46" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="G46" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H46" s="3" t="s">
+      <c r="D46" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E46" s="4" t="s">
         <v>200</v>
       </c>
+      <c r="F46" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H46" s="4" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="C47" s="4">
+      <c r="A47" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="C47" s="3">
         <v>3</v>
       </c>
-      <c r="D47" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="E47" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="F47" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="G47" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H47" s="3" t="s">
+      <c r="D47" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="F47" s="4" t="s">
         <v>205</v>
       </c>
+      <c r="G47" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H47" s="4" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="B48" s="3" t="s">
+      <c r="A48" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="C48" s="4">
+      <c r="B48" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="C48" s="3">
         <v>6</v>
       </c>
-      <c r="D48" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E48" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="F48" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="G48" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H48" s="3" t="s">
+      <c r="D48" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="F48" s="4" t="s">
         <v>209</v>
       </c>
+      <c r="G48" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H48" s="4" t="s">
+        <v>210</v>
+      </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="B49" s="3" t="s">
+      <c r="A49" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="C49" s="4">
+      <c r="B49" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="C49" s="3">
         <v>1</v>
       </c>
-      <c r="D49" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E49" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="F49" s="3" t="s">
+      <c r="D49" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E49" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="G49" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H49" s="3" t="s">
+      <c r="F49" s="4" t="s">
         <v>214</v>
       </c>
+      <c r="G49" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H49" s="4" t="s">
+        <v>215</v>
+      </c>
     </row>
   </sheetData>
-  <printOptions horizontalCentered="1" verticalCentered="1"/>
-  <pageMargins left="0.30555555555555558" right="0.30555555555555558" top="0.30555555555555558" bottom="0.30555555555555558" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="46" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" tooltip="Component" display="'Sullins" xr:uid="{968D0E8C-E264-4757-8B5B-F8729179FAA8}"/>
+    <hyperlink ref="F2" r:id="rId2" tooltip="Manufacturer" display="'QPC02SXGN-RC" xr:uid="{3A259D1A-C8D6-4A68-AF0B-F9E84B5BF698}"/>
+    <hyperlink ref="H2" r:id="rId3" tooltip="Supplier" display="'S9337-ND" xr:uid="{5A55CBB3-E246-409D-87D7-9C28414BE66F}"/>
+    <hyperlink ref="E3" r:id="rId4" tooltip="Component" display="'Panasonic" xr:uid="{EB5AC404-4900-4A80-A2F6-30827D1FF4B9}"/>
+    <hyperlink ref="F3" r:id="rId5" tooltip="Manufacturer" display="'EEEFT1V101AP" xr:uid="{C27514B6-5A42-41A1-865D-0A9933033B02}"/>
+    <hyperlink ref="H3" r:id="rId6" tooltip="Supplier" display="'PCE5016CT-ND" xr:uid="{8430A3B2-DB52-4C10-9072-5B1A7CB7F1BF}"/>
+    <hyperlink ref="E4" r:id="rId7" tooltip="Component" display="'Yageo" xr:uid="{69C69036-6429-4349-BF8F-E5A7212A5511}"/>
+    <hyperlink ref="F4" r:id="rId8" tooltip="Manufacturer" display="'CC0603KRX7R9BB104" xr:uid="{1298FC2D-C313-4A52-AD45-BEE14BBB19BB}"/>
+    <hyperlink ref="H4" r:id="rId9" tooltip="Supplier" display="'311-1344-1-ND" xr:uid="{333C80B1-69A8-4A02-8208-94AE7ACC6260}"/>
+    <hyperlink ref="E5" r:id="rId10" tooltip="Component" display="'Taiyo Yuden" xr:uid="{632E2916-E95E-4AA3-A8CD-1B5C9D5403FC}"/>
+    <hyperlink ref="F5" r:id="rId11" tooltip="Manufacturer" display="'EMK107B7105KA-T" xr:uid="{96EE8B45-599C-48BD-B1ED-C4208B5B2C9C}"/>
+    <hyperlink ref="H5" r:id="rId12" tooltip="Supplier" display="'587-1241-1-ND" xr:uid="{4C1FFDAD-BA0A-4B8C-B99A-3E053A9615EA}"/>
+    <hyperlink ref="E6" r:id="rId13" tooltip="Component" display="'TDK" xr:uid="{D9006911-2E9C-4E0A-A280-B43E3A04DD2D}"/>
+    <hyperlink ref="F6" r:id="rId14" tooltip="Manufacturer" display="'C2012X7R1A475K085AC" xr:uid="{054583CF-ED97-443D-924D-6D260563D04C}"/>
+    <hyperlink ref="H6" r:id="rId15" tooltip="Supplier" display="'445-14527-1-ND" xr:uid="{815A05C7-7215-4A04-A512-BEF88F8CB0BE}"/>
+    <hyperlink ref="E7" r:id="rId16" tooltip="Component" display="'KEMET" xr:uid="{EA44CAC7-443E-47B5-9CD0-F4A55C9D3D1D}"/>
+    <hyperlink ref="F7" r:id="rId17" tooltip="Manufacturer" display="'C1210C475K5RACTU" xr:uid="{7F8BC83B-F0A2-400B-80A4-3ED79574C53B}"/>
+    <hyperlink ref="H7" r:id="rId18" tooltip="Supplier" display="'399-6785-1-ND" xr:uid="{D8FD8B0F-A345-4FA8-A4EC-BABC05F08F96}"/>
+    <hyperlink ref="E8" r:id="rId19" tooltip="Component" display="'Kyocera AVX" xr:uid="{8D537837-0655-49CD-9FA0-E78413479153}"/>
+    <hyperlink ref="F8" r:id="rId20" tooltip="Manufacturer" display="'06035C220JAT2A" xr:uid="{2ECE4ECD-7EF1-4221-BD6F-24EE4D4CED7F}"/>
+    <hyperlink ref="H8" r:id="rId21" tooltip="Supplier" display="'478-6204-1-ND" xr:uid="{A918053C-735E-4A7D-BFCE-C4E28DA2C61F}"/>
+    <hyperlink ref="E9" r:id="rId22" tooltip="Component" display="'Molex" xr:uid="{0BB4D920-7876-457A-9717-54682FA1228F}"/>
+    <hyperlink ref="F9" r:id="rId23" tooltip="Manufacturer" display="'105017-0001" xr:uid="{0A394AC6-C695-41EA-B8EA-AC4644547172}"/>
+    <hyperlink ref="H9" r:id="rId24" tooltip="Supplier" display="'WM1399CT-ND" xr:uid="{D13FAB76-5308-43FA-975F-A95413FF43B5}"/>
+    <hyperlink ref="E10" r:id="rId25" tooltip="Component" display="'Epson" xr:uid="{1F107096-D020-4D57-BBFD-8617545B52E5}"/>
+    <hyperlink ref="F10" r:id="rId26" tooltip="Manufacturer" display="'FA-23816.0000MBC3" xr:uid="{31727DCC-3BE3-48CE-8FD4-2EFDB4A11E73}"/>
+    <hyperlink ref="H10" r:id="rId27" tooltip="Supplier" display="'SER3686CT-ND" xr:uid="{475AEC55-D8E5-43FB-BBE5-8FA9B872DADF}"/>
+    <hyperlink ref="E11" r:id="rId28" tooltip="Component" display="'MCC" xr:uid="{A3F5DABD-B806-48B9-BFFC-4A8BB3C54216}"/>
+    <hyperlink ref="F11" r:id="rId29" tooltip="Manufacturer" display="'1N4148WX-TP" xr:uid="{2114553A-8C8D-4B97-9E7D-66484D1AC910}"/>
+    <hyperlink ref="H11" r:id="rId30" tooltip="Supplier" display="'1N4148WXTPMSCT-ND" xr:uid="{9EFC2350-A0E2-4A58-9353-9946486DEFB8}"/>
+    <hyperlink ref="E12" r:id="rId31" tooltip="Component" display="'Diodes" xr:uid="{690407A6-6EA5-4F1D-A60F-00B8F4762F78}"/>
+    <hyperlink ref="F12" r:id="rId32" tooltip="Manufacturer" display="'S2BA-13-F" xr:uid="{4D39F105-18A9-44B3-AE62-7E9C529522D0}"/>
+    <hyperlink ref="H12" r:id="rId33" tooltip="Supplier" display="'S2BA-FDICT-ND" xr:uid="{FB2318FC-1CEA-4516-9823-342E78349355}"/>
+    <hyperlink ref="E13" r:id="rId34" tooltip="Component" display="'ON Semiconductor / Fairchild" xr:uid="{4E4F84F2-5185-42F0-86FD-57FAAF97E7E9}"/>
+    <hyperlink ref="F13" r:id="rId35" tooltip="Manufacturer" display="'SS24FL" xr:uid="{CBEAA36F-5830-4D52-93C0-A4F4023FEE56}"/>
+    <hyperlink ref="H13" r:id="rId36" tooltip="Supplier" display="'SS24FLCT-ND" xr:uid="{C46E322C-1B46-417B-8025-00909E55EC21}"/>
+    <hyperlink ref="E14" r:id="rId37" tooltip="Component" display="'General Instruments" xr:uid="{1D9E5376-87DA-4817-85B7-0742963064D7}"/>
+    <hyperlink ref="F14" r:id="rId38" tooltip="Manufacturer" display="'SSB44-E3/52T" xr:uid="{5AF28CF8-5933-419B-A97E-3512FD6281DB}"/>
+    <hyperlink ref="H14" r:id="rId39" tooltip="Supplier" display="'SSB44-E3/52TGICT-ND" xr:uid="{95D38656-6AA6-4DDC-B2B3-7BDFD2E8D595}"/>
+    <hyperlink ref="E15" r:id="rId40" tooltip="Component" display="'Murata" xr:uid="{C1ECC8BB-E507-4CF9-9701-6625FF1A3E11}"/>
+    <hyperlink ref="F15" r:id="rId41" tooltip="Manufacturer" display="'BLM21PG221SN1D" xr:uid="{90B91779-DFD9-4D05-B292-87A64EA558A9}"/>
+    <hyperlink ref="H15" r:id="rId42" tooltip="Supplier" display="'490-1054-1-ND" xr:uid="{6EEB8355-2529-4328-8E73-F9B2AC83A5DC}"/>
+    <hyperlink ref="E16" r:id="rId43" tooltip="Component" display="'Bourns" xr:uid="{9FD1DD88-6857-42CA-90E6-F766FDE4D2AE}"/>
+    <hyperlink ref="F16" r:id="rId44" tooltip="Manufacturer" display="'SRN6045TA-4R7M" xr:uid="{BEF8AF03-CBCD-4C4A-98AE-BBE459A01DB8}"/>
+    <hyperlink ref="H16" r:id="rId45" tooltip="Supplier" display="'SRN6045TA-4R7MCT-ND" xr:uid="{54306C89-52F4-4D65-9CD7-6CB8B45E777B}"/>
+    <hyperlink ref="E17" r:id="rId46" tooltip="Component" display="'Bourns" xr:uid="{F1D17519-FF3E-4330-82EE-62EC46F3288E}"/>
+    <hyperlink ref="F17" r:id="rId47" tooltip="Manufacturer" display="'SRN6045TA-330M" xr:uid="{9AA163F8-932E-4015-86F5-EC9038EC11CF}"/>
+    <hyperlink ref="H17" r:id="rId48" tooltip="Supplier" display="'SRN6045TA-330MCT-ND" xr:uid="{461EC537-6F35-435E-8400-80A041C28154}"/>
+    <hyperlink ref="E18" r:id="rId49" tooltip="Component" display="'Memory Protection Devices" xr:uid="{1B593CEE-DAF5-4688-AA27-C3937BBA52C1}"/>
+    <hyperlink ref="F18" r:id="rId50" tooltip="Manufacturer" display="'BK-6013" xr:uid="{60360EE8-7494-49C3-A559-51FD8158D85A}"/>
+    <hyperlink ref="H18" r:id="rId51" tooltip="Supplier" display="'BK-6013-ND" xr:uid="{FD38A260-870C-4E3C-AEC5-FD3678D9B772}"/>
+    <hyperlink ref="E19" tooltip="Component" display="'Generic Header" xr:uid="{29336B69-1CD4-4E8E-A0BE-3C72933D2340}"/>
+    <hyperlink ref="F19" tooltip="Manufacturer" display="'" xr:uid="{6DEA9FAE-5659-4EFF-A8D7-3C5166CC3BD1}"/>
+    <hyperlink ref="H19" tooltip="Supplier" display="'" xr:uid="{ED4B894D-C366-4BCC-9330-F8218667A3ED}"/>
+    <hyperlink ref="E20" tooltip="Component" display="'Generic Header" xr:uid="{00B90512-B31D-4406-B8E0-964A4C5B338B}"/>
+    <hyperlink ref="F20" tooltip="Manufacturer" display="'" xr:uid="{F8DA7A3D-4DC1-43E8-BB51-0D5906E6C348}"/>
+    <hyperlink ref="H20" tooltip="Supplier" display="'" xr:uid="{01F0A89F-5AAA-4D17-9507-18EDBBF3A9F3}"/>
+    <hyperlink ref="E21" tooltip="Component" display="'Generic Header" xr:uid="{5D1B5577-A906-4BC8-9526-C10D6E5BA67D}"/>
+    <hyperlink ref="F21" tooltip="Manufacturer" display="'" xr:uid="{CA733CFC-BDB7-4E7A-94C6-44DF33A85A9E}"/>
+    <hyperlink ref="H21" tooltip="Supplier" display="'" xr:uid="{145E4BBA-7D5A-43E3-9E80-B3205413A393}"/>
+    <hyperlink ref="E22" tooltip="Component" display="'Generic Header" xr:uid="{905E99FA-710A-4505-8E77-A2EF2A7929B0}"/>
+    <hyperlink ref="F22" tooltip="Manufacturer" display="'" xr:uid="{70451FC8-6C2D-4812-8C13-4C0A93C84023}"/>
+    <hyperlink ref="H22" tooltip="Supplier" display="'" xr:uid="{AAC3B58B-7D3F-499A-9F65-2F658455081C}"/>
+    <hyperlink ref="E23" tooltip="Component" display="'Generic Header" xr:uid="{F9EDDF67-8A2B-478C-B87C-2A7D07DC1B83}"/>
+    <hyperlink ref="F23" tooltip="Manufacturer" display="'" xr:uid="{BEC91BDC-BBFB-4ACC-95A0-BAFD3F5431EF}"/>
+    <hyperlink ref="H23" tooltip="Supplier" display="'" xr:uid="{935056A1-CE1B-4BDE-B441-E7EEBD8BEBC9}"/>
+    <hyperlink ref="E24" tooltip="Component" display="'Generic Header" xr:uid="{75214B9D-5C8C-4B68-95B2-6AE2C59341C1}"/>
+    <hyperlink ref="F24" tooltip="Manufacturer" display="'" xr:uid="{46E6C33C-42FC-4AA0-B535-4301C002B270}"/>
+    <hyperlink ref="H24" tooltip="Supplier" display="'" xr:uid="{D5528D46-88B5-408E-BE92-D43D3969F9CA}"/>
+    <hyperlink ref="E25" tooltip="Component" display="'Generic Header" xr:uid="{144B5E20-0049-486B-A2BD-DB0CA54BA8FB}"/>
+    <hyperlink ref="F25" tooltip="Manufacturer" display="'" xr:uid="{5C532C4F-EF9E-4509-9658-CE22C27200E4}"/>
+    <hyperlink ref="H25" tooltip="Supplier" display="'" xr:uid="{52D0C4F8-F307-4CB6-BC57-057435321817}"/>
+    <hyperlink ref="E26" tooltip="Component" display="'Generic Header" xr:uid="{3A884513-4FA0-4277-818B-89BED84FB8A5}"/>
+    <hyperlink ref="F26" tooltip="Manufacturer" display="'" xr:uid="{32CD951C-B778-4FDF-9F9C-4DAA3380CD83}"/>
+    <hyperlink ref="H26" tooltip="Supplier" display="'" xr:uid="{999E6854-65B1-41F3-8E9D-A64431F1E0C5}"/>
+    <hyperlink ref="E27" r:id="rId52" tooltip="Component" display="'Microchip" xr:uid="{3195AFA5-BF60-474E-9247-0A04960ECEB9}"/>
+    <hyperlink ref="F27" r:id="rId53" tooltip="Manufacturer" display="'ATMEGA16U2-MU" xr:uid="{4DECF356-C660-440B-81A6-0AE732444232}"/>
+    <hyperlink ref="H27" r:id="rId54" tooltip="Supplier" display="'ATMEGA16U2-MU-ND" xr:uid="{2E6C2AAB-E9FF-428D-9F88-5240F4A27355}"/>
+    <hyperlink ref="E28" r:id="rId55" tooltip="Component" display="'Microchip / Atmel" xr:uid="{9251B13A-FB49-4B24-85A1-2ADC4ED5C302}"/>
+    <hyperlink ref="F28" r:id="rId56" tooltip="Manufacturer" display="'ATMEGA2560-16AU" xr:uid="{48BBAEBC-9AEF-44C6-8355-A6D27B429448}"/>
+    <hyperlink ref="H28" r:id="rId57" tooltip="Supplier" display="'ATMEGA2560-16AU-ND" xr:uid="{3A301433-A086-4086-AB1C-D6F09429CCA5}"/>
+    <hyperlink ref="E29" r:id="rId58" tooltip="Component" display="'Alpha &amp; Omega Semiconductor" xr:uid="{EF1C8527-9956-48DE-B8EA-4F93D2D0B467}"/>
+    <hyperlink ref="F29" r:id="rId59" tooltip="Manufacturer" display="'AOZ1282CI" xr:uid="{2ABBC3F4-1036-40BA-A635-49E19839C750}"/>
+    <hyperlink ref="H29" r:id="rId60" tooltip="Supplier" display="'785-1613-1-ND" xr:uid="{0A9E099A-475C-4722-8378-F3CE1BB3531A}"/>
+    <hyperlink ref="E30" r:id="rId61" tooltip="Component" display="'Alpha &amp; Omega Semiconductor" xr:uid="{1BDFE91B-A8F4-408B-BFB1-3C3C4C6E0375}"/>
+    <hyperlink ref="F30" r:id="rId62" tooltip="Manufacturer" display="'AOZ1284PI" xr:uid="{52B3D08F-EC52-427D-A6E7-E0288AD40927}"/>
+    <hyperlink ref="H30" r:id="rId63" tooltip="Supplier" display="'785-1689-1-ND" xr:uid="{782A92D1-1D1E-473D-B497-68999C367C60}"/>
+    <hyperlink ref="E31" r:id="rId64" tooltip="Component" display="'Vishay Lite-On" xr:uid="{731552BA-797D-4A2A-ADDF-DAA870F3C01F}"/>
+    <hyperlink ref="F31" r:id="rId65" tooltip="Manufacturer" display="'LTST-C190KGKT" xr:uid="{D11BEF18-A6EF-4895-A93D-0AFB577E5F56}"/>
+    <hyperlink ref="H31" r:id="rId66" tooltip="Supplier" display="'160-1435-2-ND" xr:uid="{855D88D3-76B1-4276-BFBD-2F4E0F34210F}"/>
+    <hyperlink ref="E32" r:id="rId67" tooltip="Component" display="'Vishay Lite-On" xr:uid="{144EFC4E-4110-4556-A3F5-ECB8EEB85DAB}"/>
+    <hyperlink ref="F32" r:id="rId68" tooltip="Manufacturer" display="'LTST-C190KSKT" xr:uid="{FFFA9BDB-3C43-4A5B-96F6-67130A1A0514}"/>
+    <hyperlink ref="H32" r:id="rId69" tooltip="Supplier" display="'160-1437-1-ND" xr:uid="{60BA805D-4A97-4DD4-93BF-A03B72F92DB9}"/>
+    <hyperlink ref="E33" r:id="rId70" tooltip="Component" display="'Nexperia" xr:uid="{5BB9ED0E-804F-4FE6-8E71-D4FC5C2F9106}"/>
+    <hyperlink ref="F33" r:id="rId71" tooltip="Manufacturer" display="'BUK9Y21-40E,115" xr:uid="{172D9B76-7170-4EEC-8C25-7D9C59410462}"/>
+    <hyperlink ref="H33" r:id="rId72" tooltip="Supplier" display="'1727-1123-1-ND" xr:uid="{B4915611-75D4-4549-BB8A-8FC6C254C1AD}"/>
+    <hyperlink ref="E34" r:id="rId73" tooltip="Component" display="'Nexperia" xr:uid="{D7874A4D-D663-42E2-95CD-246F12E14A21}"/>
+    <hyperlink ref="F34" r:id="rId74" tooltip="Manufacturer" display="'PSMN1R8-40YLC,115" xr:uid="{610AA18B-8B6C-4B70-B47E-A80FE0124201}"/>
+    <hyperlink ref="H34" r:id="rId75" tooltip="Supplier" display="'1727-1052-1-ND" xr:uid="{E47EAD35-97B1-452C-8C73-F912E11BF6C8}"/>
+    <hyperlink ref="E35" r:id="rId76" tooltip="Component" display="'Bel" xr:uid="{893B7A6B-056B-4E50-86FC-CD1743A729F7}"/>
+    <hyperlink ref="F35" r:id="rId77" tooltip="Manufacturer" display="'0ZCM0020FF2G" xr:uid="{F81CFA7F-8F7E-4C11-A6D7-A7877D343565}"/>
+    <hyperlink ref="H35" r:id="rId78" tooltip="Supplier" display="'507-1821-1-ND" xr:uid="{6FEAB7CD-EAE9-4923-99F5-C07A98E806D4}"/>
+    <hyperlink ref="E36" r:id="rId79" tooltip="Component" display="'Yageo" xr:uid="{52CFA0DA-AF8D-4C6D-A5F8-4B9AC118123A}"/>
+    <hyperlink ref="F36" r:id="rId80" tooltip="Manufacturer" display="'RC0603FR-071KL" xr:uid="{F7508EC3-2047-45BE-81C7-C9C0A49DFA07}"/>
+    <hyperlink ref="H36" r:id="rId81" tooltip="Supplier" display="'311-1.00KHRCT-ND" xr:uid="{C8D5BEDE-8466-4F7A-AE02-AB2DD0332593}"/>
+    <hyperlink ref="E37" r:id="rId82" tooltip="Component" display="'Yageo" xr:uid="{C4EBE395-3476-42EB-9EBC-60DEB505145B}"/>
+    <hyperlink ref="F37" r:id="rId83" tooltip="Manufacturer" display="'RC0603FR-071ML" xr:uid="{8697BB15-9216-40E4-996A-9EC03CE178DA}"/>
+    <hyperlink ref="H37" r:id="rId84" tooltip="Supplier" display="'311-1.00MHRDKR-ND" xr:uid="{A6B015D8-9497-4742-B000-C0FC3B97DB8D}"/>
+    <hyperlink ref="E38" r:id="rId85" tooltip="Component" display="'Yageo" xr:uid="{899C85BC-10C9-4C44-AA78-830E832678A3}"/>
+    <hyperlink ref="F38" r:id="rId86" tooltip="Manufacturer" display="'RC0603FR-074K7L" xr:uid="{15D37BA0-C1D2-41EF-B3B6-19C519B1383F}"/>
+    <hyperlink ref="H38" r:id="rId87" tooltip="Supplier" display="'311-4.70KHRCT-ND" xr:uid="{0BF9F661-B9DE-42CD-B3B9-845E287B71EC}"/>
+    <hyperlink ref="E39" r:id="rId88" tooltip="Component" display="'Yageo Phycomp" xr:uid="{06EEF875-9E1E-418B-B720-EE26A5870E4B}"/>
+    <hyperlink ref="F39" r:id="rId89" tooltip="Manufacturer" display="'RC0603FR-0710KL" xr:uid="{831667F8-F910-4175-BCC2-6869B07B3CD5}"/>
+    <hyperlink ref="H39" r:id="rId90" tooltip="Supplier" display="'311-10.0KHRCT-ND" xr:uid="{9478D5F6-84E9-4412-BE3D-5194463FE0DD}"/>
+    <hyperlink ref="E40" r:id="rId91" tooltip="Component" display="'Yageo" xr:uid="{E7B060BA-597B-4ED8-8595-23124A463F88}"/>
+    <hyperlink ref="F40" r:id="rId92" tooltip="Manufacturer" display="'RC0603FR-0722RL" xr:uid="{3C02D33D-D6D5-4FA8-BC3D-2FFF05278355}"/>
+    <hyperlink ref="H40" r:id="rId93" tooltip="Supplier" display="'311-22.0HRCT-ND" xr:uid="{14069EB5-8B29-4C8A-82DC-26145ABB3363}"/>
+    <hyperlink ref="E41" r:id="rId94" tooltip="Component" display="'Yageo" xr:uid="{60143F7D-8080-4765-843C-BFD3B5FEF581}"/>
+    <hyperlink ref="F41" r:id="rId95" tooltip="Manufacturer" display="'RC0603FR-0754K9L" xr:uid="{F2ED1F02-EBDA-40B1-8337-92D7542B94AE}"/>
+    <hyperlink ref="H41" r:id="rId96" tooltip="Supplier" display="'311-54.9KHRCT-ND" xr:uid="{3676D8C4-E489-4601-BD98-63AF90227B19}"/>
+    <hyperlink ref="E42" r:id="rId97" tooltip="Component" display="'Yageo" xr:uid="{4072A16D-8B62-4705-A9AA-DDA7FD8E6F98}"/>
+    <hyperlink ref="F42" r:id="rId98" tooltip="Manufacturer" display="'RC0603FR-07100KL" xr:uid="{3BC8DF01-5911-466A-A1C3-E4A64245B266}"/>
+    <hyperlink ref="H42" r:id="rId99" tooltip="Supplier" display="'311-100KHRCT-ND" xr:uid="{32A21A1F-C00A-4366-B2F5-9051560263EE}"/>
+    <hyperlink ref="E43" r:id="rId100" tooltip="Component" display="'Yageo" xr:uid="{C94E959A-EC2B-4165-800C-2A19C2E3B4D3}"/>
+    <hyperlink ref="F43" r:id="rId101" tooltip="Manufacturer" display="'RC0603FR-07140KL" xr:uid="{A21527CE-6578-4CC0-9652-BBFD95A3F052}"/>
+    <hyperlink ref="H43" r:id="rId102" tooltip="Supplier" display="'311-140KHRCT-ND" xr:uid="{77240F23-9D50-4B6C-9D6B-F36414A9A2B6}"/>
+    <hyperlink ref="E44" r:id="rId103" tooltip="Component" display="'Wurth Electronics" xr:uid="{50C81BEA-33A3-42AE-A1BE-2A145BD6DB88}"/>
+    <hyperlink ref="F44" r:id="rId104" tooltip="Manufacturer" display="'416131160803" xr:uid="{DF58EE5F-E402-4445-BF08-AEE160161C56}"/>
+    <hyperlink ref="H44" r:id="rId105" tooltip="Supplier" display="'732-3853-1-ND" xr:uid="{393EC610-B2F1-4BF8-84E1-B089717B95BA}"/>
+    <hyperlink ref="E45" r:id="rId106" tooltip="Component" display="'APEM" xr:uid="{332FDA72-75C8-4E67-A6FC-E965354EEFA4}"/>
+    <hyperlink ref="F45" r:id="rId107" tooltip="Manufacturer" display="'MJTP1106SATR" xr:uid="{A8D580BF-0966-42A4-908B-B104724BA267}"/>
+    <hyperlink ref="H45" r:id="rId108" tooltip="Supplier" display="'679-2396-1-ND" xr:uid="{DC5284EC-944D-4965-9597-B793DD971B63}"/>
+    <hyperlink ref="E46" r:id="rId109" tooltip="Component" display="'Phoenix Contact" xr:uid="{D96B4B63-4B17-438E-ABF9-A5D310D8AD1B}"/>
+    <hyperlink ref="F46" r:id="rId110" tooltip="Manufacturer" display="'MKDS1/2-3,5" xr:uid="{8D256E76-4545-480F-A24A-1F0421756DEF}"/>
+    <hyperlink ref="H46" r:id="rId111" tooltip="Supplier" display="'277-5719-ND" xr:uid="{BBCE262C-DF8C-4C38-A0E9-C8A5B3CE7E74}"/>
+    <hyperlink ref="E47" r:id="rId112" tooltip="Component" display="'Phoenix Contact" xr:uid="{C2F0362B-9B05-4A1A-9F50-FF6071721A39}"/>
+    <hyperlink ref="F47" r:id="rId113" tooltip="Manufacturer" display="'1935776" xr:uid="{CE0C2560-5A42-405A-AC1D-21C03E147C60}"/>
+    <hyperlink ref="H47" r:id="rId114" tooltip="Supplier" display="'277-6405-ND" xr:uid="{32127689-5B92-43B3-9111-45BCB41E9EBD}"/>
+    <hyperlink ref="E48" r:id="rId115" tooltip="Component" display="'Phoenix Contact" xr:uid="{77922A95-0152-4759-9934-B4740485314B}"/>
+    <hyperlink ref="F48" r:id="rId116" tooltip="Manufacturer" display="'MKDS1/4-3,5" xr:uid="{B75E61A6-F0F9-4F3C-B94E-B34FC649A5F3}"/>
+    <hyperlink ref="H48" r:id="rId117" tooltip="Supplier" display="'277-5744-ND" xr:uid="{AAD59821-C808-4EB8-BC90-DC9992EE939E}"/>
+    <hyperlink ref="E49" r:id="rId118" tooltip="Component" display="'STMicroelectronics" xr:uid="{EF65047E-7CC6-4485-A9C4-5327B0C3D4F8}"/>
+    <hyperlink ref="F49" r:id="rId119" tooltip="Manufacturer" display="'USBLC6-4SC6" xr:uid="{2BF9253A-F67F-409F-B793-EA7D1E862D03}"/>
+    <hyperlink ref="H49" r:id="rId120" tooltip="Supplier" display="'497-4492-1-ND" xr:uid="{FC5E01C6-24FA-4BD0-B60D-5D3AF2F5493E}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId121"/>
 </worksheet>
 </file>
</xml_diff>